<commit_message>
Comments and Changed To County Median
</commit_message>
<xml_diff>
--- a/indicator_definitions_updated.xlsx
+++ b/indicator_definitions_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e053c53d61b8413/Documents/GitHub/CED-Housing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{02B99954-6413-40CD-AB95-61560ED0D563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5832DE8D-9188-45B2-87D6-2189660F51AA}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{02B99954-6413-40CD-AB95-61560ED0D563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2121874-7DDD-4D39-BB58-918F42E67B91}"/>
   <bookViews>
-    <workbookView xWindow="-8988" yWindow="7956" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="192">
   <si>
     <t>Group</t>
   </si>
@@ -577,6 +577,30 @@
   </si>
   <si>
     <t>ACS Vacancy Rate</t>
+  </si>
+  <si>
+    <t>PrcntChangeFMR2016_2020</t>
+  </si>
+  <si>
+    <t>PrcntChangeFMR2020_2022</t>
+  </si>
+  <si>
+    <t>PrcntChangeEmployWage2016_2020</t>
+  </si>
+  <si>
+    <t>PrcntChangeEmployTotal2016_2020</t>
+  </si>
+  <si>
+    <t>Percent Change of the Fair Market Rent of a 2 Bedroom Apartment from 2016 to 2020</t>
+  </si>
+  <si>
+    <t>Percent Change of the Fair Market Rent of a 2 Bedroom Apartment from 2020 to 2022</t>
+  </si>
+  <si>
+    <t>Percent Change of Wage and Salaried Employment from 2016 to 2020</t>
+  </si>
+  <si>
+    <t>Percent Change of Total and Salaried Employment from 2016 to 2020</t>
   </si>
 </sst>
 </file>
@@ -903,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2320,6 +2344,122 @@
         <v>8</v>
       </c>
     </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" t="s">
+        <v>187</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>